<commit_message>
Added latest Q4 FY24 quarter for AMD
</commit_message>
<xml_diff>
--- a/data/AMD.xlsx
+++ b/data/AMD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tngam\projects\python\stock-kpi-plot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE47EB66-E36D-422D-A588-D3BEB014ED94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65465006-11EC-4085-8E15-DB98073EC0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="11490" windowWidth="38380" windowHeight="20970" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38380" windowHeight="20880" xr2:uid="{847D2414-6927-4BEE-9896-7F31C50B6E3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Report Date</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Q1 FY23</t>
+  </si>
+  <si>
+    <t>Q4 FY24</t>
   </si>
 </sst>
 </file>
@@ -451,7 +454,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -460,8 +463,8 @@
     <col min="2" max="3" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.08984375" customWidth="1"/>
     <col min="5" max="5" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
@@ -491,6 +494,9 @@
       <c r="H1" t="s">
         <v>4</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -517,7 +523,9 @@
       <c r="H2" s="1">
         <v>45563</v>
       </c>
-      <c r="I2" s="1"/>
+      <c r="I2" s="1">
+        <v>45654</v>
+      </c>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -549,6 +557,9 @@
       <c r="H3">
         <v>3549</v>
       </c>
+      <c r="I3">
+        <v>3859</v>
+      </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
@@ -577,6 +588,9 @@
       <c r="H4">
         <v>1881</v>
       </c>
+      <c r="I4">
+        <v>2313</v>
+      </c>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
@@ -605,6 +619,9 @@
       <c r="H5">
         <v>462</v>
       </c>
+      <c r="I5">
+        <v>563</v>
+      </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
     </row>
@@ -632,6 +649,9 @@
       </c>
       <c r="H6">
         <v>927</v>
+      </c>
+      <c r="I6">
+        <v>923</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>

</xml_diff>